<commit_message>
Final edits before Ledpin heat control
</commit_message>
<xml_diff>
--- a/CurrentCatheter.xlsx
+++ b/CurrentCatheter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Materials</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
   <si>
     <t>Soft, black</t>
@@ -425,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,7 +462,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -483,7 +477,7 @@
         <v>1.98</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -491,7 +485,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -506,12 +500,12 @@
         <v>1.17</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -526,22 +520,6 @@
         <v>1.17</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>